<commit_message>
Fix and test missing remark
</commit_message>
<xml_diff>
--- a/packages/timeseries-parsers/lib/multi-params/__tests__/test-files/missing-remark.xlsx
+++ b/packages/timeseries-parsers/lib/multi-params/__tests__/test-files/missing-remark.xlsx
@@ -4270,11 +4270,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
     <numFmt numFmtId="60" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="61" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -4622,9 +4621,7 @@
       <left style="hair">
         <color indexed="8"/>
       </left>
-      <right>
-        <color indexed="8"/>
-      </right>
+      <right/>
       <top style="hair">
         <color indexed="8"/>
       </top>
@@ -4634,9 +4631,7 @@
       <diagonal/>
     </border>
     <border>
-      <left>
-        <color indexed="8"/>
-      </left>
+      <left/>
       <right style="hair">
         <color indexed="8"/>
       </right>
@@ -4682,7 +4677,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -4905,9 +4900,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="61" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -5106,9 +5098,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -5172,12 +5164,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst>
           <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
@@ -5188,7 +5180,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -5215,10 +5207,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -5457,17 +5449,17 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -5745,7 +5737,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -5772,10 +5764,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -17628,7 +17620,7 @@
     <row r="11" ht="13.65" customHeight="1">
       <c r="A11" s="58"/>
       <c r="B11" s="59">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C11" s="60"/>
       <c r="D11" s="45"/>
@@ -29683,7 +29675,7 @@
       <formula1>"valeur brute,minimum,maximum,moyenne,médiane,différence d’index,autre"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:I4">
-      <formula1>"seconde,minute,15 minutes,heure,jour,mois,trimestre,année,autre"</formula1>
+      <formula1>"seconde,minute,15min,heure,jour,mois,trimestre,année,autre,15min,15 minutes"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:I5">
       <formula1>"µS/cm,degrés Celsius,L/s,m³/h,m³,m NGR,mg/L,autre"</formula1>
@@ -29747,7 +29739,7 @@
         <v>1299</v>
       </c>
       <c r="C2" t="s" s="35">
-        <v>30</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s" s="36">
         <v>16</v>
@@ -29969,11 +29961,11 @@
     </row>
     <row r="13" ht="13.65" customHeight="1">
       <c r="A13" s="63">
-        <v>36526</v>
+        <v>45658</v>
       </c>
       <c r="B13" s="64"/>
       <c r="C13" s="73">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="D13" s="66"/>
       <c r="E13" s="67"/>
@@ -29984,8 +29976,8 @@
       <c r="J13" s="71"/>
     </row>
     <row r="14" ht="13.65" customHeight="1">
-      <c r="A14" s="74">
-        <v>36557</v>
+      <c r="A14" s="63">
+        <v>45659</v>
       </c>
       <c r="B14" s="64"/>
       <c r="C14" s="65"/>
@@ -41985,7 +41977,7 @@
       <formula1>"valeur brute,minimum,maximum,moyenne,médiane,différence d’index,autre"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:I4">
-      <formula1>"seconde,minute,15 minutes,heure,jour,mois,trimestre,année,autre"</formula1>
+      <formula1>"seconde,minute,15min,heure,jour,mois,trimestre,année,autre"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:I5">
       <formula1>"µS/cm,degrés Celsius,L/s,m³/h,m³,m NGR,mg/L,autre"</formula1>
@@ -42008,11 +42000,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="11.6719" style="75" customWidth="1"/>
-    <col min="2" max="2" width="18.5" style="75" customWidth="1"/>
-    <col min="3" max="9" width="16.6719" style="75" customWidth="1"/>
-    <col min="10" max="10" width="21.1719" style="75" customWidth="1"/>
-    <col min="11" max="16384" width="11.5" style="75" customWidth="1"/>
+    <col min="1" max="1" width="11.6719" style="74" customWidth="1"/>
+    <col min="2" max="2" width="18.5" style="74" customWidth="1"/>
+    <col min="3" max="9" width="16.6719" style="74" customWidth="1"/>
+    <col min="10" max="10" width="21.1719" style="74" customWidth="1"/>
+    <col min="11" max="16384" width="11.5" style="74" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -54281,7 +54273,7 @@
       <formula1>"valeur brute,minimum,maximum,moyenne,médiane,différence d’index,autre"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:I4">
-      <formula1>"seconde,minute,15 minutes,heure,jour,mois,trimestre,année,autre"</formula1>
+      <formula1>"seconde,minute,15min,heure,jour,mois,trimestre,année,autre"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:I5">
       <formula1>"µS/cm,degrés Celsius,L/s,m³/h,m³,m NGR,mg/L,autre"</formula1>
@@ -54304,15 +54296,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.8516" style="76" customWidth="1"/>
-    <col min="2" max="2" width="18.5" style="76" customWidth="1"/>
-    <col min="3" max="9" width="17.5" style="76" customWidth="1"/>
-    <col min="10" max="10" width="21.1719" style="76" customWidth="1"/>
-    <col min="11" max="16384" width="11.5" style="76" customWidth="1"/>
+    <col min="1" max="1" width="10.8516" style="75" customWidth="1"/>
+    <col min="2" max="2" width="18.5" style="75" customWidth="1"/>
+    <col min="3" max="9" width="17.5" style="75" customWidth="1"/>
+    <col min="10" max="10" width="21.1719" style="75" customWidth="1"/>
+    <col min="11" max="16384" width="11.5" style="75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" s="77"/>
+      <c r="A1" s="76"/>
       <c r="B1" s="30"/>
       <c r="C1" t="s" s="31">
         <v>1291</v>
@@ -54338,7 +54330,7 @@
       <c r="J1" s="32"/>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" t="s" s="78">
+      <c r="A2" t="s" s="77">
         <v>1298</v>
       </c>
       <c r="B2" t="s" s="34">
@@ -54368,7 +54360,7 @@
       <c r="J2" s="42"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="79"/>
+      <c r="A3" s="78"/>
       <c r="B3" t="s" s="34">
         <v>1300</v>
       </c>
@@ -54396,7 +54388,7 @@
       <c r="J3" s="42"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="79"/>
+      <c r="A4" s="78"/>
       <c r="B4" t="s" s="34">
         <v>1301</v>
       </c>
@@ -54424,7 +54416,7 @@
       <c r="J4" s="42"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="79"/>
+      <c r="A5" s="78"/>
       <c r="B5" t="s" s="34">
         <v>1302</v>
       </c>
@@ -54452,7 +54444,7 @@
       <c r="J5" s="42"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="79"/>
+      <c r="A6" s="78"/>
       <c r="B6" t="s" s="34">
         <v>1303</v>
       </c>
@@ -54466,7 +54458,7 @@
       <c r="J6" s="42"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="79"/>
+      <c r="A7" s="78"/>
       <c r="B7" t="s" s="34">
         <v>1304</v>
       </c>
@@ -54480,7 +54472,7 @@
       <c r="J7" s="42"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="79"/>
+      <c r="A8" s="78"/>
       <c r="B8" t="s" s="34">
         <v>1305</v>
       </c>
@@ -54494,7 +54486,7 @@
       <c r="J8" s="42"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="79"/>
+      <c r="A9" s="78"/>
       <c r="B9" t="s" s="34">
         <v>1306</v>
       </c>
@@ -54508,7 +54500,7 @@
       <c r="J9" s="42"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="80"/>
+      <c r="A10" s="79"/>
       <c r="B10" t="s" s="34">
         <v>1307</v>
       </c>
@@ -66577,7 +66569,7 @@
       <formula1>"valeur brute,minimum,maximum,moyenne,médiane,différence d’index,autre"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:I4">
-      <formula1>"seconde,minute,15 minutes,heure,jour,mois,trimestre,année,autre"</formula1>
+      <formula1>"seconde,minute,15min,heure,jour,mois,trimestre,année,autre"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:I5">
       <formula1>"µS/cm,degrés Celsius,L/s,m³/h,m³,m NGR,mg/L,autre"</formula1>

</xml_diff>